<commit_message>
practice set fow working with excels
</commit_message>
<xml_diff>
--- a/Working_With_Excels/Book1.xlsx
+++ b/Working_With_Excels/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium_Practice_Code_learning\Selenium_practice_code\Working_With_Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69164149-1898-4983-ADB2-DAF7A9D85098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46CDAFB-0839-4F51-BC5C-B164F09EEB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{035A2F95-9037-4B64-B159-3F3589AE9F6D}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9120" xr2:uid="{035A2F95-9037-4B64-B159-3F3589AE9F6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -25,33 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t xml:space="preserve">Greeting </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communication </t>
-  </si>
-  <si>
-    <t>ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abc </t>
-  </si>
-  <si>
-    <t>efg</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>abc1</t>
-  </si>
-  <si>
-    <t>efg1</t>
-  </si>
-  <si>
-    <t>xyz1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">sr no </t>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastname </t>
+  </si>
+  <si>
+    <t xml:space="preserve">age </t>
+  </si>
+  <si>
+    <t xml:space="preserve">lavanya </t>
+  </si>
+  <si>
+    <t>ghadge</t>
+  </si>
+  <si>
+    <t>roshan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanjay </t>
+  </si>
+  <si>
+    <t>vijaya</t>
   </si>
 </sst>
 </file>
@@ -75,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -83,28 +83,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,56 +403,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4068C45-94FF-4F78-B6C0-9D36357CF7D2}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
+      <c r="D5">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>